<commit_message>
Error reading Federica dataset
</commit_message>
<xml_diff>
--- a/extdata/Froc.xlsx
+++ b/extdata/Froc.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1097B511-B3AC-8549-88F0-6C4BA52852A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E304FF6-F4A7-2A4E-8A8F-D125BD8B4574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="660" windowWidth="33940" windowHeight="21540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TP" sheetId="3" r:id="rId1"/>
-    <sheet name="FP" sheetId="2" r:id="rId2"/>
-    <sheet name="Truth" sheetId="1" r:id="rId3"/>
+    <sheet name="LL" sheetId="3" r:id="rId1"/>
+    <sheet name="NL" sheetId="2" r:id="rId2"/>
+    <sheet name="TRUTH" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>CaseID</t>
   </si>
@@ -47,35 +47,20 @@
     <t>ModalityID</t>
   </si>
   <si>
-    <t>TP_Rating</t>
-  </si>
-  <si>
-    <t>FP_Rating</t>
-  </si>
-  <si>
     <t>ReaderID</t>
   </si>
   <si>
-    <t>Paradigm</t>
+    <t>LLRating</t>
   </si>
   <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>1,3,4,5</t>
-  </si>
-  <si>
-    <t>FROC</t>
-  </si>
-  <si>
-    <t>FCTRL</t>
+    <t>NLRating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -96,6 +81,11 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -134,7 +124,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -151,10 +141,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -510,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E737"/>
   <sheetViews>
-    <sheetView topLeftCell="A670" zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -524,7 +517,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -535,8 +528,8 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -13069,19 +13062,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D568"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A121" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="4" width="8.83203125" style="2"/>
-    <col min="5" max="16384" width="8.83203125" style="7"/>
+    <col min="5" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -13089,8 +13082,8 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
+      <c r="D1" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -21047,10 +21040,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F243"/>
+  <dimension ref="A1:C243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21058,12 +21051,9 @@
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21073,17 +21063,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -21093,17 +21074,8 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -21113,17 +21085,8 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -21133,15 +21096,8 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -21151,15 +21107,8 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -21169,15 +21118,8 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -21187,15 +21129,8 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -21205,15 +21140,8 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -21223,15 +21151,8 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -21241,15 +21162,8 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -21259,15 +21173,8 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -21277,15 +21184,8 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -21295,15 +21195,8 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -21313,14 +21206,8 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -21330,14 +21217,8 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -21347,14 +21228,8 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -21364,14 +21239,8 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -21381,14 +21250,8 @@
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -21398,14 +21261,8 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -21415,14 +21272,8 @@
       <c r="C20" s="1">
         <v>1</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -21432,14 +21283,8 @@
       <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -21449,14 +21294,8 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -21466,14 +21305,8 @@
       <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -21483,14 +21316,8 @@
       <c r="C24" s="1">
         <v>1</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -21500,14 +21327,8 @@
       <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -21517,14 +21338,8 @@
       <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -21534,14 +21349,8 @@
       <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -21551,14 +21360,8 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -21568,14 +21371,8 @@
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -21585,14 +21382,8 @@
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -21602,14 +21393,8 @@
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -21619,14 +21404,8 @@
       <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -21636,14 +21415,8 @@
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -21653,14 +21426,8 @@
       <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -21670,14 +21437,8 @@
       <c r="C35" s="1">
         <v>1</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -21687,14 +21448,8 @@
       <c r="C36" s="1">
         <v>1</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -21704,14 +21459,8 @@
       <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -21721,14 +21470,8 @@
       <c r="C38" s="1">
         <v>1</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -21738,14 +21481,8 @@
       <c r="C39" s="1">
         <v>1</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -21755,14 +21492,8 @@
       <c r="C40" s="1">
         <v>1</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -21772,14 +21503,8 @@
       <c r="C41" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -21789,14 +21514,8 @@
       <c r="C42" s="1">
         <v>1</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -21806,14 +21525,8 @@
       <c r="C43" s="1">
         <v>1</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -21823,14 +21536,8 @@
       <c r="C44" s="1">
         <v>1</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -21840,14 +21547,8 @@
       <c r="C45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -21857,14 +21558,8 @@
       <c r="C46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -21874,14 +21569,8 @@
       <c r="C47" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -21891,14 +21580,8 @@
       <c r="C48" s="1">
         <v>1</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -21908,14 +21591,8 @@
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -21925,14 +21602,8 @@
       <c r="C50" s="1">
         <v>1</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -21942,14 +21613,8 @@
       <c r="C51" s="1">
         <v>1</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -21959,14 +21624,8 @@
       <c r="C52" s="1">
         <v>1</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -21976,14 +21635,8 @@
       <c r="C53" s="1">
         <v>1</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -21993,14 +21646,8 @@
       <c r="C54" s="1">
         <v>1</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -22010,14 +21657,8 @@
       <c r="C55" s="1">
         <v>1</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -22027,14 +21668,8 @@
       <c r="C56" s="1">
         <v>1</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -22044,14 +21679,8 @@
       <c r="C57" s="1">
         <v>0.5</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
         <v>55</v>
       </c>
@@ -22061,14 +21690,8 @@
       <c r="C58" s="1">
         <v>0.5</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
         <v>56</v>
       </c>
@@ -22078,14 +21701,8 @@
       <c r="C59" s="1">
         <v>0.5</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -22095,14 +21712,8 @@
       <c r="C60" s="1">
         <v>0.5</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -22112,14 +21723,8 @@
       <c r="C61" s="1">
         <v>1</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -22129,14 +21734,8 @@
       <c r="C62" s="1">
         <v>1</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -22146,14 +21745,8 @@
       <c r="C63" s="1">
         <v>0.5</v>
       </c>
-      <c r="D63" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
         <v>59</v>
       </c>
@@ -22163,14 +21756,8 @@
       <c r="C64" s="1">
         <v>0.5</v>
       </c>
-      <c r="D64" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
         <v>60</v>
       </c>
@@ -22180,14 +21767,8 @@
       <c r="C65" s="1">
         <v>1</v>
       </c>
-      <c r="D65" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
         <v>61</v>
       </c>
@@ -22197,14 +21778,8 @@
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
         <v>62</v>
       </c>
@@ -22214,14 +21789,8 @@
       <c r="C67" s="1">
         <v>1</v>
       </c>
-      <c r="D67" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
         <v>63</v>
       </c>
@@ -22231,14 +21800,8 @@
       <c r="C68" s="1">
         <v>1</v>
       </c>
-      <c r="D68" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
         <v>64</v>
       </c>
@@ -22248,14 +21811,8 @@
       <c r="C69" s="1">
         <v>1</v>
       </c>
-      <c r="D69" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1">
         <v>65</v>
       </c>
@@ -22265,14 +21822,8 @@
       <c r="C70" s="1">
         <v>1</v>
       </c>
-      <c r="D70" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="1">
         <v>66</v>
       </c>
@@ -22282,14 +21833,8 @@
       <c r="C71" s="1">
         <v>1</v>
       </c>
-      <c r="D71" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
         <v>67</v>
       </c>
@@ -22299,14 +21844,8 @@
       <c r="C72" s="1">
         <v>1</v>
       </c>
-      <c r="D72" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="1">
         <v>68</v>
       </c>
@@ -22316,14 +21855,8 @@
       <c r="C73" s="1">
         <v>0.5</v>
       </c>
-      <c r="D73" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
         <v>68</v>
       </c>
@@ -22333,14 +21866,8 @@
       <c r="C74" s="1">
         <v>0.5</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
         <v>69</v>
       </c>
@@ -22350,14 +21877,8 @@
       <c r="C75" s="1">
         <v>0.5</v>
       </c>
-      <c r="D75" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
         <v>69</v>
       </c>
@@ -22367,14 +21888,8 @@
       <c r="C76" s="1">
         <v>0.5</v>
       </c>
-      <c r="D76" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
         <v>70</v>
       </c>
@@ -22384,14 +21899,8 @@
       <c r="C77" s="1">
         <v>1</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
         <v>71</v>
       </c>
@@ -22401,14 +21910,8 @@
       <c r="C78" s="1">
         <v>1</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
         <v>72</v>
       </c>
@@ -22418,14 +21921,8 @@
       <c r="C79" s="1">
         <v>1</v>
       </c>
-      <c r="D79" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
         <v>73</v>
       </c>
@@ -22435,14 +21932,8 @@
       <c r="C80" s="1">
         <v>0.5</v>
       </c>
-      <c r="D80" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>73</v>
       </c>
@@ -22452,14 +21943,8 @@
       <c r="C81" s="1">
         <v>0.5</v>
       </c>
-      <c r="D81" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>74</v>
       </c>
@@ -22469,14 +21954,8 @@
       <c r="C82" s="1">
         <v>0.5</v>
       </c>
-      <c r="D82" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>74</v>
       </c>
@@ -22486,14 +21965,8 @@
       <c r="C83" s="1">
         <v>0.5</v>
       </c>
-      <c r="D83" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>75</v>
       </c>
@@ -22503,14 +21976,8 @@
       <c r="C84" s="1">
         <v>0.5</v>
       </c>
-      <c r="D84" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>75</v>
       </c>
@@ -22520,14 +21987,8 @@
       <c r="C85" s="1">
         <v>0.5</v>
       </c>
-      <c r="D85" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
         <v>76</v>
       </c>
@@ -22537,14 +21998,8 @@
       <c r="C86" s="1">
         <v>0.5</v>
       </c>
-      <c r="D86" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
         <v>76</v>
       </c>
@@ -22554,14 +22009,8 @@
       <c r="C87" s="1">
         <v>0.5</v>
       </c>
-      <c r="D87" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
         <v>77</v>
       </c>
@@ -22571,14 +22020,8 @@
       <c r="C88" s="1">
         <v>0.5</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
         <v>77</v>
       </c>
@@ -22588,14 +22031,8 @@
       <c r="C89" s="1">
         <v>0.5</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>78</v>
       </c>
@@ -22605,14 +22042,8 @@
       <c r="C90" s="1">
         <v>0.5</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>78</v>
       </c>
@@ -22622,14 +22053,8 @@
       <c r="C91" s="1">
         <v>0.5</v>
       </c>
-      <c r="D91" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>79</v>
       </c>
@@ -22639,14 +22064,8 @@
       <c r="C92" s="1">
         <v>1</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>80</v>
       </c>
@@ -22656,14 +22075,8 @@
       <c r="C93" s="1">
         <v>0.5</v>
       </c>
-      <c r="D93" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>80</v>
       </c>
@@ -22673,14 +22086,8 @@
       <c r="C94" s="1">
         <v>0.5</v>
       </c>
-      <c r="D94" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>81</v>
       </c>
@@ -22690,14 +22097,8 @@
       <c r="C95" s="1">
         <v>0.5</v>
       </c>
-      <c r="D95" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
         <v>81</v>
       </c>
@@ -22707,14 +22108,8 @@
       <c r="C96" s="1">
         <v>0.5</v>
       </c>
-      <c r="D96" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
         <v>82</v>
       </c>
@@ -22724,14 +22119,8 @@
       <c r="C97" s="1">
         <v>0.5</v>
       </c>
-      <c r="D97" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
         <v>82</v>
       </c>
@@ -22741,14 +22130,8 @@
       <c r="C98" s="1">
         <v>0.5</v>
       </c>
-      <c r="D98" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
         <v>83</v>
       </c>
@@ -22758,14 +22141,8 @@
       <c r="C99" s="1">
         <v>0.5</v>
       </c>
-      <c r="D99" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
         <v>83</v>
       </c>
@@ -22775,14 +22152,8 @@
       <c r="C100" s="1">
         <v>0.5</v>
       </c>
-      <c r="D100" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
         <v>84</v>
       </c>
@@ -22792,14 +22163,8 @@
       <c r="C101" s="1">
         <v>0.33</v>
       </c>
-      <c r="D101" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
         <v>84</v>
       </c>
@@ -22809,14 +22174,8 @@
       <c r="C102" s="1">
         <v>0.33</v>
       </c>
-      <c r="D102" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
         <v>84</v>
       </c>
@@ -22826,14 +22185,8 @@
       <c r="C103" s="1">
         <v>0.33</v>
       </c>
-      <c r="D103" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
         <v>85</v>
       </c>
@@ -22843,14 +22196,8 @@
       <c r="C104" s="1">
         <v>0.5</v>
       </c>
-      <c r="D104" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
         <v>85</v>
       </c>
@@ -22860,14 +22207,8 @@
       <c r="C105" s="1">
         <v>0.5</v>
       </c>
-      <c r="D105" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
         <v>86</v>
       </c>
@@ -22877,14 +22218,8 @@
       <c r="C106" s="1">
         <v>0.5</v>
       </c>
-      <c r="D106" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
         <v>86</v>
       </c>
@@ -22894,14 +22229,8 @@
       <c r="C107" s="1">
         <v>0.5</v>
       </c>
-      <c r="D107" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
         <v>87</v>
       </c>
@@ -22911,14 +22240,8 @@
       <c r="C108" s="1">
         <v>0.5</v>
       </c>
-      <c r="D108" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
         <v>87</v>
       </c>
@@ -22928,14 +22251,8 @@
       <c r="C109" s="1">
         <v>0.5</v>
       </c>
-      <c r="D109" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
         <v>88</v>
       </c>
@@ -22945,14 +22262,8 @@
       <c r="C110" s="1">
         <v>0.5</v>
       </c>
-      <c r="D110" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1">
         <v>88</v>
       </c>
@@ -22962,14 +22273,8 @@
       <c r="C111" s="1">
         <v>0.5</v>
       </c>
-      <c r="D111" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" s="1">
         <v>89</v>
       </c>
@@ -22979,14 +22284,8 @@
       <c r="C112" s="1">
         <v>0.5</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1">
         <v>89</v>
       </c>
@@ -22996,14 +22295,8 @@
       <c r="C113" s="1">
         <v>0.5</v>
       </c>
-      <c r="D113" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1">
         <v>90</v>
       </c>
@@ -23013,14 +22306,8 @@
       <c r="C114" s="1">
         <v>0.33</v>
       </c>
-      <c r="D114" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1">
         <v>90</v>
       </c>
@@ -23030,14 +22317,8 @@
       <c r="C115" s="1">
         <v>0.33</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1">
         <v>90</v>
       </c>
@@ -23047,14 +22328,8 @@
       <c r="C116" s="1">
         <v>0.33</v>
       </c>
-      <c r="D116" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1">
         <v>91</v>
       </c>
@@ -23064,14 +22339,8 @@
       <c r="C117" s="1">
         <v>0.33</v>
       </c>
-      <c r="D117" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1">
         <v>91</v>
       </c>
@@ -23081,14 +22350,8 @@
       <c r="C118" s="1">
         <v>0.33</v>
       </c>
-      <c r="D118" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1">
         <v>91</v>
       </c>
@@ -23098,14 +22361,8 @@
       <c r="C119" s="1">
         <v>0.33</v>
       </c>
-      <c r="D119" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1">
         <v>92</v>
       </c>
@@ -23115,14 +22372,8 @@
       <c r="C120" s="1">
         <v>0.33</v>
       </c>
-      <c r="D120" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A121" s="1">
         <v>92</v>
       </c>
@@ -23132,14 +22383,8 @@
       <c r="C121" s="1">
         <v>0.33</v>
       </c>
-      <c r="D121" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1">
         <v>92</v>
       </c>
@@ -23149,14 +22394,8 @@
       <c r="C122" s="1">
         <v>0.33</v>
       </c>
-      <c r="D122" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1">
         <v>93</v>
       </c>
@@ -23166,14 +22405,8 @@
       <c r="C123" s="1">
         <v>0.33</v>
       </c>
-      <c r="D123" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1">
         <v>93</v>
       </c>
@@ -23183,14 +22416,8 @@
       <c r="C124" s="1">
         <v>0.33</v>
       </c>
-      <c r="D124" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A125" s="1">
         <v>93</v>
       </c>
@@ -23200,14 +22427,8 @@
       <c r="C125" s="1">
         <v>0.33</v>
       </c>
-      <c r="D125" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1">
         <v>94</v>
       </c>
@@ -23217,14 +22438,8 @@
       <c r="C126" s="1">
         <v>0.33</v>
       </c>
-      <c r="D126" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
         <v>94</v>
       </c>
@@ -23234,14 +22449,8 @@
       <c r="C127" s="1">
         <v>0.33</v>
       </c>
-      <c r="D127" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E127" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1">
         <v>94</v>
       </c>
@@ -23251,14 +22460,8 @@
       <c r="C128" s="1">
         <v>0.33</v>
       </c>
-      <c r="D128" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E128" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A129" s="1">
         <v>95</v>
       </c>
@@ -23268,14 +22471,8 @@
       <c r="C129" s="1">
         <v>0.33</v>
       </c>
-      <c r="D129" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E129" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1">
         <v>95</v>
       </c>
@@ -23285,14 +22482,8 @@
       <c r="C130" s="1">
         <v>0.33</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E130" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1">
         <v>95</v>
       </c>
@@ -23302,14 +22493,8 @@
       <c r="C131" s="1">
         <v>0.33</v>
       </c>
-      <c r="D131" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1">
         <v>96</v>
       </c>
@@ -23319,14 +22504,8 @@
       <c r="C132" s="1">
         <v>0.33</v>
       </c>
-      <c r="D132" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E132" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1">
         <v>96</v>
       </c>
@@ -23336,14 +22515,8 @@
       <c r="C133" s="1">
         <v>0.33</v>
       </c>
-      <c r="D133" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1">
         <v>96</v>
       </c>
@@ -23353,14 +22526,8 @@
       <c r="C134" s="1">
         <v>0.33</v>
       </c>
-      <c r="D134" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1">
         <v>97</v>
       </c>
@@ -23370,14 +22537,8 @@
       <c r="C135" s="1">
         <v>0.33</v>
       </c>
-      <c r="D135" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1">
         <v>97</v>
       </c>
@@ -23387,14 +22548,8 @@
       <c r="C136" s="1">
         <v>0.33</v>
       </c>
-      <c r="D136" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1">
         <v>97</v>
       </c>
@@ -23404,14 +22559,8 @@
       <c r="C137" s="1">
         <v>0.33</v>
       </c>
-      <c r="D137" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E137" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1">
         <v>98</v>
       </c>
@@ -23421,14 +22570,8 @@
       <c r="C138" s="1">
         <v>0.33</v>
       </c>
-      <c r="D138" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1">
         <v>98</v>
       </c>
@@ -23438,14 +22581,8 @@
       <c r="C139" s="1">
         <v>0.33</v>
       </c>
-      <c r="D139" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1">
         <v>98</v>
       </c>
@@ -23455,14 +22592,8 @@
       <c r="C140" s="1">
         <v>0.33</v>
       </c>
-      <c r="D140" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E140" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1">
         <v>99</v>
       </c>
@@ -23472,14 +22603,8 @@
       <c r="C141" s="1">
         <v>0.33</v>
       </c>
-      <c r="D141" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E141" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1">
         <v>99</v>
       </c>
@@ -23489,14 +22614,8 @@
       <c r="C142" s="1">
         <v>0.33</v>
       </c>
-      <c r="D142" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E142" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="1">
         <v>99</v>
       </c>
@@ -23506,14 +22625,8 @@
       <c r="C143" s="1">
         <v>0.33</v>
       </c>
-      <c r="D143" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E143" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1">
         <v>100</v>
       </c>
@@ -23523,14 +22636,8 @@
       <c r="C144" s="1">
         <v>0</v>
       </c>
-      <c r="D144" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E144" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1">
         <v>101</v>
       </c>
@@ -23540,14 +22647,8 @@
       <c r="C145" s="1">
         <v>0</v>
       </c>
-      <c r="D145" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E145" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1">
         <v>102</v>
       </c>
@@ -23557,14 +22658,8 @@
       <c r="C146" s="1">
         <v>0</v>
       </c>
-      <c r="D146" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E146" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1">
         <v>103</v>
       </c>
@@ -23574,14 +22669,8 @@
       <c r="C147" s="1">
         <v>0</v>
       </c>
-      <c r="D147" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E147" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1">
         <v>104</v>
       </c>
@@ -23591,14 +22680,8 @@
       <c r="C148" s="1">
         <v>0</v>
       </c>
-      <c r="D148" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="1">
         <v>105</v>
       </c>
@@ -23608,14 +22691,8 @@
       <c r="C149" s="1">
         <v>0</v>
       </c>
-      <c r="D149" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E149" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1">
         <v>106</v>
       </c>
@@ -23625,14 +22702,8 @@
       <c r="C150" s="1">
         <v>0</v>
       </c>
-      <c r="D150" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E150" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1">
         <v>107</v>
       </c>
@@ -23642,14 +22713,8 @@
       <c r="C151" s="1">
         <v>0</v>
       </c>
-      <c r="D151" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E151" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A152" s="1">
         <v>108</v>
       </c>
@@ -23659,14 +22724,8 @@
       <c r="C152" s="1">
         <v>0</v>
       </c>
-      <c r="D152" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E152" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1">
         <v>109</v>
       </c>
@@ -23676,14 +22735,8 @@
       <c r="C153" s="1">
         <v>0</v>
       </c>
-      <c r="D153" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E153" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1">
         <v>110</v>
       </c>
@@ -23693,14 +22746,8 @@
       <c r="C154" s="1">
         <v>0</v>
       </c>
-      <c r="D154" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E154" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1">
         <v>111</v>
       </c>
@@ -23710,14 +22757,8 @@
       <c r="C155" s="1">
         <v>0</v>
       </c>
-      <c r="D155" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E155" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A156" s="1">
         <v>112</v>
       </c>
@@ -23727,14 +22768,8 @@
       <c r="C156" s="1">
         <v>0</v>
       </c>
-      <c r="D156" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E156" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A157" s="1">
         <v>113</v>
       </c>
@@ -23744,14 +22779,8 @@
       <c r="C157" s="1">
         <v>0</v>
       </c>
-      <c r="D157" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E157" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A158" s="1">
         <v>114</v>
       </c>
@@ -23761,14 +22790,8 @@
       <c r="C158" s="1">
         <v>0</v>
       </c>
-      <c r="D158" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A159" s="1">
         <v>115</v>
       </c>
@@ -23778,14 +22801,8 @@
       <c r="C159" s="1">
         <v>0</v>
       </c>
-      <c r="D159" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E159" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A160" s="1">
         <v>116</v>
       </c>
@@ -23795,14 +22812,8 @@
       <c r="C160" s="1">
         <v>0</v>
       </c>
-      <c r="D160" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E160" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A161" s="1">
         <v>117</v>
       </c>
@@ -23812,14 +22823,8 @@
       <c r="C161" s="1">
         <v>0</v>
       </c>
-      <c r="D161" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E161" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A162" s="1">
         <v>118</v>
       </c>
@@ -23829,14 +22834,8 @@
       <c r="C162" s="1">
         <v>0</v>
       </c>
-      <c r="D162" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A163" s="1">
         <v>119</v>
       </c>
@@ -23846,14 +22845,8 @@
       <c r="C163" s="1">
         <v>0</v>
       </c>
-      <c r="D163" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E163" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A164" s="1">
         <v>120</v>
       </c>
@@ -23863,14 +22856,8 @@
       <c r="C164" s="1">
         <v>0</v>
       </c>
-      <c r="D164" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E164" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A165" s="1">
         <v>121</v>
       </c>
@@ -23880,14 +22867,8 @@
       <c r="C165" s="1">
         <v>0</v>
       </c>
-      <c r="D165" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E165" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A166" s="1">
         <v>122</v>
       </c>
@@ -23897,14 +22878,8 @@
       <c r="C166" s="1">
         <v>0</v>
       </c>
-      <c r="D166" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E166" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A167" s="1">
         <v>123</v>
       </c>
@@ -23914,14 +22889,8 @@
       <c r="C167" s="1">
         <v>0</v>
       </c>
-      <c r="D167" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E167" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A168" s="1">
         <v>124</v>
       </c>
@@ -23931,14 +22900,8 @@
       <c r="C168" s="1">
         <v>0</v>
       </c>
-      <c r="D168" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E168" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" s="1">
         <v>125</v>
       </c>
@@ -23948,14 +22911,8 @@
       <c r="C169" s="1">
         <v>0</v>
       </c>
-      <c r="D169" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E169" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A170" s="1">
         <v>126</v>
       </c>
@@ -23965,14 +22922,8 @@
       <c r="C170" s="1">
         <v>0</v>
       </c>
-      <c r="D170" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E170" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" s="1">
         <v>127</v>
       </c>
@@ -23982,14 +22933,8 @@
       <c r="C171" s="1">
         <v>0</v>
       </c>
-      <c r="D171" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E171" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A172" s="1">
         <v>128</v>
       </c>
@@ -23999,14 +22944,8 @@
       <c r="C172" s="1">
         <v>0</v>
       </c>
-      <c r="D172" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E172" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A173" s="1">
         <v>129</v>
       </c>
@@ -24016,14 +22955,8 @@
       <c r="C173" s="1">
         <v>0</v>
       </c>
-      <c r="D173" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E173" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A174" s="1">
         <v>130</v>
       </c>
@@ -24033,14 +22966,8 @@
       <c r="C174" s="1">
         <v>0</v>
       </c>
-      <c r="D174" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E174" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A175" s="1">
         <v>131</v>
       </c>
@@ -24050,14 +22977,8 @@
       <c r="C175" s="1">
         <v>0</v>
       </c>
-      <c r="D175" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E175" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1">
         <v>132</v>
       </c>
@@ -24067,14 +22988,8 @@
       <c r="C176" s="1">
         <v>0</v>
       </c>
-      <c r="D176" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E176" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1">
         <v>133</v>
       </c>
@@ -24084,14 +22999,8 @@
       <c r="C177" s="1">
         <v>0</v>
       </c>
-      <c r="D177" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E177" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1">
         <v>134</v>
       </c>
@@ -24101,14 +23010,8 @@
       <c r="C178" s="1">
         <v>0</v>
       </c>
-      <c r="D178" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E178" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1">
         <v>135</v>
       </c>
@@ -24118,14 +23021,8 @@
       <c r="C179" s="1">
         <v>0</v>
       </c>
-      <c r="D179" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E179" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A180" s="1">
         <v>136</v>
       </c>
@@ -24135,14 +23032,8 @@
       <c r="C180" s="1">
         <v>0</v>
       </c>
-      <c r="D180" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E180" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A181" s="1">
         <v>137</v>
       </c>
@@ -24152,14 +23043,8 @@
       <c r="C181" s="1">
         <v>0</v>
       </c>
-      <c r="D181" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E181" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A182" s="1">
         <v>138</v>
       </c>
@@ -24169,14 +23054,8 @@
       <c r="C182" s="1">
         <v>0</v>
       </c>
-      <c r="D182" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E182" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A183" s="1">
         <v>139</v>
       </c>
@@ -24186,14 +23065,8 @@
       <c r="C183" s="1">
         <v>0</v>
       </c>
-      <c r="D183" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E183" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1">
         <v>140</v>
       </c>
@@ -24203,14 +23076,8 @@
       <c r="C184" s="1">
         <v>0</v>
       </c>
-      <c r="D184" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E184" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A185" s="1">
         <v>141</v>
       </c>
@@ -24220,14 +23087,8 @@
       <c r="C185" s="1">
         <v>0</v>
       </c>
-      <c r="D185" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E185" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A186" s="1">
         <v>142</v>
       </c>
@@ -24237,14 +23098,8 @@
       <c r="C186" s="1">
         <v>0</v>
       </c>
-      <c r="D186" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E186" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A187" s="1">
         <v>143</v>
       </c>
@@ -24254,14 +23109,8 @@
       <c r="C187" s="1">
         <v>0</v>
       </c>
-      <c r="D187" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E187" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A188" s="1">
         <v>144</v>
       </c>
@@ -24271,14 +23120,8 @@
       <c r="C188" s="1">
         <v>0</v>
       </c>
-      <c r="D188" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E188" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A189" s="1">
         <v>145</v>
       </c>
@@ -24288,14 +23131,8 @@
       <c r="C189" s="1">
         <v>0</v>
       </c>
-      <c r="D189" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E189" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A190" s="1">
         <v>146</v>
       </c>
@@ -24305,14 +23142,8 @@
       <c r="C190" s="1">
         <v>0</v>
       </c>
-      <c r="D190" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E190" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A191" s="1">
         <v>147</v>
       </c>
@@ -24322,14 +23153,8 @@
       <c r="C191" s="1">
         <v>0</v>
       </c>
-      <c r="D191" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E191" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A192" s="1">
         <v>148</v>
       </c>
@@ -24339,14 +23164,8 @@
       <c r="C192" s="1">
         <v>0</v>
       </c>
-      <c r="D192" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E192" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A193" s="1">
         <v>149</v>
       </c>
@@ -24356,14 +23175,8 @@
       <c r="C193" s="1">
         <v>0</v>
       </c>
-      <c r="D193" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E193" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A194" s="1">
         <v>150</v>
       </c>
@@ -24373,14 +23186,8 @@
       <c r="C194" s="1">
         <v>0</v>
       </c>
-      <c r="D194" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E194" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A195" s="1">
         <v>151</v>
       </c>
@@ -24390,14 +23197,8 @@
       <c r="C195" s="1">
         <v>0</v>
       </c>
-      <c r="D195" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E195" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A196" s="1">
         <v>152</v>
       </c>
@@ -24407,14 +23208,8 @@
       <c r="C196" s="1">
         <v>0</v>
       </c>
-      <c r="D196" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E196" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A197" s="1">
         <v>153</v>
       </c>
@@ -24424,14 +23219,8 @@
       <c r="C197" s="1">
         <v>0</v>
       </c>
-      <c r="D197" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E197" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A198" s="1">
         <v>154</v>
       </c>
@@ -24441,14 +23230,8 @@
       <c r="C198" s="1">
         <v>0</v>
       </c>
-      <c r="D198" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E198" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A199" s="1">
         <v>155</v>
       </c>
@@ -24458,14 +23241,8 @@
       <c r="C199" s="1">
         <v>0</v>
       </c>
-      <c r="D199" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E199" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A200" s="1">
         <v>156</v>
       </c>
@@ -24475,14 +23252,8 @@
       <c r="C200" s="1">
         <v>0</v>
       </c>
-      <c r="D200" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E200" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A201" s="1">
         <v>157</v>
       </c>
@@ -24492,14 +23263,8 @@
       <c r="C201" s="1">
         <v>0</v>
       </c>
-      <c r="D201" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E201" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A202" s="1">
         <v>158</v>
       </c>
@@ -24509,14 +23274,8 @@
       <c r="C202" s="1">
         <v>0</v>
       </c>
-      <c r="D202" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E202" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A203" s="1">
         <v>159</v>
       </c>
@@ -24526,14 +23285,8 @@
       <c r="C203" s="1">
         <v>0</v>
       </c>
-      <c r="D203" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E203" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A204" s="1">
         <v>160</v>
       </c>
@@ -24543,14 +23296,8 @@
       <c r="C204" s="1">
         <v>0</v>
       </c>
-      <c r="D204" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E204" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A205" s="1">
         <v>161</v>
       </c>
@@ -24560,14 +23307,8 @@
       <c r="C205" s="1">
         <v>0</v>
       </c>
-      <c r="D205" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E205" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A206" s="1">
         <v>162</v>
       </c>
@@ -24577,14 +23318,8 @@
       <c r="C206" s="1">
         <v>0</v>
       </c>
-      <c r="D206" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E206" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A207" s="1">
         <v>163</v>
       </c>
@@ -24594,14 +23329,8 @@
       <c r="C207" s="1">
         <v>0</v>
       </c>
-      <c r="D207" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E207" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A208" s="1">
         <v>164</v>
       </c>
@@ -24611,14 +23340,8 @@
       <c r="C208" s="1">
         <v>0</v>
       </c>
-      <c r="D208" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E208" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A209" s="1">
         <v>165</v>
       </c>
@@ -24628,14 +23351,8 @@
       <c r="C209" s="1">
         <v>0</v>
       </c>
-      <c r="D209" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E209" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A210" s="1">
         <v>166</v>
       </c>
@@ -24645,14 +23362,8 @@
       <c r="C210" s="1">
         <v>0</v>
       </c>
-      <c r="D210" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E210" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A211" s="1">
         <v>167</v>
       </c>
@@ -24662,14 +23373,8 @@
       <c r="C211" s="1">
         <v>0</v>
       </c>
-      <c r="D211" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E211" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A212" s="1">
         <v>168</v>
       </c>
@@ -24679,14 +23384,8 @@
       <c r="C212" s="1">
         <v>0</v>
       </c>
-      <c r="D212" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E212" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A213" s="1">
         <v>169</v>
       </c>
@@ -24696,14 +23395,8 @@
       <c r="C213" s="1">
         <v>0</v>
       </c>
-      <c r="D213" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E213" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A214" s="1">
         <v>170</v>
       </c>
@@ -24713,14 +23406,8 @@
       <c r="C214" s="1">
         <v>0</v>
       </c>
-      <c r="D214" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E214" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A215" s="1">
         <v>171</v>
       </c>
@@ -24730,14 +23417,8 @@
       <c r="C215" s="1">
         <v>0</v>
       </c>
-      <c r="D215" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E215" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A216" s="1">
         <v>172</v>
       </c>
@@ -24747,14 +23428,8 @@
       <c r="C216" s="1">
         <v>0</v>
       </c>
-      <c r="D216" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E216" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A217" s="1">
         <v>173</v>
       </c>
@@ -24764,14 +23439,8 @@
       <c r="C217" s="1">
         <v>0</v>
       </c>
-      <c r="D217" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E217" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A218" s="1">
         <v>174</v>
       </c>
@@ -24781,14 +23450,8 @@
       <c r="C218" s="1">
         <v>0</v>
       </c>
-      <c r="D218" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E218" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A219" s="1">
         <v>175</v>
       </c>
@@ -24798,14 +23461,8 @@
       <c r="C219" s="1">
         <v>0</v>
       </c>
-      <c r="D219" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E219" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A220" s="1">
         <v>176</v>
       </c>
@@ -24815,14 +23472,8 @@
       <c r="C220" s="1">
         <v>0</v>
       </c>
-      <c r="D220" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E220" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A221" s="1">
         <v>177</v>
       </c>
@@ -24832,14 +23483,8 @@
       <c r="C221" s="1">
         <v>0</v>
       </c>
-      <c r="D221" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E221" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A222" s="1">
         <v>178</v>
       </c>
@@ -24849,14 +23494,8 @@
       <c r="C222" s="1">
         <v>0</v>
       </c>
-      <c r="D222" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E222" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A223" s="1">
         <v>179</v>
       </c>
@@ -24866,14 +23505,8 @@
       <c r="C223" s="1">
         <v>0</v>
       </c>
-      <c r="D223" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E223" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A224" s="1">
         <v>180</v>
       </c>
@@ -24883,14 +23516,8 @@
       <c r="C224" s="1">
         <v>0</v>
       </c>
-      <c r="D224" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E224" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A225" s="1">
         <v>181</v>
       </c>
@@ -24900,14 +23527,8 @@
       <c r="C225" s="1">
         <v>0</v>
       </c>
-      <c r="D225" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E225" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A226" s="1">
         <v>182</v>
       </c>
@@ -24917,14 +23538,8 @@
       <c r="C226" s="1">
         <v>0</v>
       </c>
-      <c r="D226" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E226" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A227" s="1">
         <v>183</v>
       </c>
@@ -24934,14 +23549,8 @@
       <c r="C227" s="1">
         <v>0</v>
       </c>
-      <c r="D227" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E227" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A228" s="1">
         <v>184</v>
       </c>
@@ -24951,14 +23560,8 @@
       <c r="C228" s="1">
         <v>0</v>
       </c>
-      <c r="D228" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E228" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A229" s="1">
         <v>185</v>
       </c>
@@ -24968,14 +23571,8 @@
       <c r="C229" s="1">
         <v>0</v>
       </c>
-      <c r="D229" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E229" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A230" s="1">
         <v>186</v>
       </c>
@@ -24985,14 +23582,8 @@
       <c r="C230" s="1">
         <v>0</v>
       </c>
-      <c r="D230" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E230" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A231" s="1">
         <v>187</v>
       </c>
@@ -25002,14 +23593,8 @@
       <c r="C231" s="1">
         <v>0</v>
       </c>
-      <c r="D231" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E231" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A232" s="1">
         <v>188</v>
       </c>
@@ -25019,14 +23604,8 @@
       <c r="C232" s="1">
         <v>0</v>
       </c>
-      <c r="D232" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E232" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A233" s="1">
         <v>189</v>
       </c>
@@ -25036,14 +23615,8 @@
       <c r="C233" s="1">
         <v>0</v>
       </c>
-      <c r="D233" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E233" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A234" s="1">
         <v>190</v>
       </c>
@@ -25053,14 +23626,8 @@
       <c r="C234" s="1">
         <v>0</v>
       </c>
-      <c r="D234" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E234" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A235" s="1">
         <v>191</v>
       </c>
@@ -25070,14 +23637,8 @@
       <c r="C235" s="1">
         <v>0</v>
       </c>
-      <c r="D235" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E235" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A236" s="1">
         <v>192</v>
       </c>
@@ -25087,14 +23648,8 @@
       <c r="C236" s="1">
         <v>0</v>
       </c>
-      <c r="D236" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E236" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A237" s="1">
         <v>193</v>
       </c>
@@ -25104,14 +23659,8 @@
       <c r="C237" s="1">
         <v>0</v>
       </c>
-      <c r="D237" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E237" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A238" s="1">
         <v>194</v>
       </c>
@@ -25121,14 +23670,8 @@
       <c r="C238" s="1">
         <v>0</v>
       </c>
-      <c r="D238" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E238" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A239" s="1">
         <v>195</v>
       </c>
@@ -25138,14 +23681,8 @@
       <c r="C239" s="1">
         <v>0</v>
       </c>
-      <c r="D239" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E239" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A240" s="1">
         <v>196</v>
       </c>
@@ -25155,14 +23692,8 @@
       <c r="C240" s="1">
         <v>0</v>
       </c>
-      <c r="D240" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E240" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A241" s="1">
         <v>197</v>
       </c>
@@ -25172,14 +23703,8 @@
       <c r="C241" s="1">
         <v>0</v>
       </c>
-      <c r="D241" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E241" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A242" s="1">
         <v>198</v>
       </c>
@@ -25189,14 +23714,8 @@
       <c r="C242" s="1">
         <v>0</v>
       </c>
-      <c r="D242" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E242" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A243" s="1">
         <v>199</v>
       </c>
@@ -25205,12 +23724,6 @@
       </c>
       <c r="C243" s="1">
         <v>0</v>
-      </c>
-      <c r="D243" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E243" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed read of Federica dataset
</commit_message>
<xml_diff>
--- a/extdata/Froc.xlsx
+++ b/extdata/Froc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E304FF6-F4A7-2A4E-8A8F-D125BD8B4574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDACAA-D3EA-294E-8917-6E0D389BD9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="500" windowWidth="21180" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LL" sheetId="3" r:id="rId1"/>
@@ -13062,8 +13062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D568"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21042,8 +21042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C243"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1048576"/>
+    <sheetView topLeftCell="A235" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A243" sqref="A243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>